<commit_message>
task 3 and 4
</commit_message>
<xml_diff>
--- a/Domaci-OMP/Izvestaj/t2.xlsx
+++ b/Domaci-OMP/Izvestaj/t2.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racicaleksa/Projects/Semestar-7/MUPS/Domaci-OMP/Izvestaj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\el190235d\Desktop\MUPS\domaci\dom1\MUPS\Domaci-OMP\Izvestaj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EB9F9096-EDB1-C842-8D5D-4E060C3EE697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E6CBF0-6D84-4CDF-BA54-CA8FB3A2E3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prime_parallel" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -591,6 +594,931 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>prime_parallel!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total_Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>prime_parallel!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>prime_parallel!$H$2:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13.929233999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.432354999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0759080000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3304079999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE5E-4734-8243-AC96B967FF2B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="661306095"/>
+        <c:axId val="661307743"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="661306095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="661307743"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="661307743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="661306095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4877F72E-C394-46F2-89A8-88560CEE3DF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="prime_parallel"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="H1" t="str">
+            <v>Total_Time</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>1</v>
+          </cell>
+          <cell r="H2">
+            <v>6.3830000000000012E-2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>2</v>
+          </cell>
+          <cell r="H3">
+            <v>2.7930000000000003E-2</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="G4">
+            <v>4</v>
+          </cell>
+          <cell r="H4">
+            <v>1.5756999999999997E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="G5">
+            <v>8</v>
+          </cell>
+          <cell r="H5">
+            <v>8.6709999999999964E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -887,16 +1815,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -916,7 +1844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -937,7 +1865,7 @@
         <v>13.929233999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -958,7 +1886,7 @@
         <v>10.432354999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -979,7 +1907,7 @@
         <v>6.0759080000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1000,7 +1928,7 @@
         <v>3.3304079999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1014,7 +1942,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1028,7 +1956,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1042,7 +1970,7 @@
         <v>6.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1056,7 +1984,7 @@
         <v>1.9000000000000001E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1070,7 +1998,7 @@
         <v>5.1E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1084,7 +2012,7 @@
         <v>1.8200000000000001E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1098,7 +2026,7 @@
         <v>6.2299999999999996E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1112,7 +2040,7 @@
         <v>2.248E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1126,7 +2054,7 @@
         <v>2.14E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1140,7 +2068,7 @@
         <v>4.9699999999999996E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1154,7 +2082,7 @@
         <v>1.9678000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1168,7 +2096,7 @@
         <v>6.8513000000000004E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1182,7 +2110,7 @@
         <v>0.25462699999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1196,7 +2124,7 @@
         <v>0.95669599999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1210,7 +2138,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1224,7 +2152,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1238,7 +2166,7 @@
         <v>3.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1252,7 +2180,7 @@
         <v>2.0079999999999998E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1266,7 +2194,7 @@
         <v>0.14937700000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1280,7 +2208,7 @@
         <v>12.198358000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1294,7 +2222,7 @@
         <v>3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1308,7 +2236,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1322,7 +2250,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1336,7 +2264,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1350,7 +2278,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1364,7 +2292,7 @@
         <v>1.07E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1378,7 +2306,7 @@
         <v>1.366E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1392,7 +2320,7 @@
         <v>1.8065000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1406,7 +2334,7 @@
         <v>0.25012200000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1420,7 +2348,7 @@
         <v>8.2000000000000001E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1434,7 +2362,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1448,7 +2376,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1462,7 +2390,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1476,7 +2404,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1490,7 +2418,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1504,7 +2432,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1518,7 +2446,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1532,7 +2460,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1546,7 +2474,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1560,7 +2488,7 @@
         <v>7.8999999999999996E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1574,7 +2502,7 @@
         <v>2.7799999999999998E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1588,7 +2516,7 @@
         <v>1.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1602,7 +2530,7 @@
         <v>3.6150000000000002E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1616,7 +2544,7 @@
         <v>1.3546000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2</v>
       </c>
@@ -1630,7 +2558,7 @@
         <v>4.9840000000000002E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2</v>
       </c>
@@ -1644,7 +2572,7 @@
         <v>0.186721</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2</v>
       </c>
@@ -1658,7 +2586,7 @@
         <v>0.702322</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2</v>
       </c>
@@ -1672,7 +2600,7 @@
         <v>5.5999999999999999E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2</v>
       </c>
@@ -1686,7 +2614,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2</v>
       </c>
@@ -1700,7 +2628,7 @@
         <v>2.6999999999999999E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2</v>
       </c>
@@ -1714,7 +2642,7 @@
         <v>1.4760000000000001E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2</v>
       </c>
@@ -1728,7 +2656,7 @@
         <v>0.112108</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1742,7 +2670,7 @@
         <v>9.1601979999999994</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1756,7 +2684,7 @@
         <v>4.5000000000000003E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2</v>
       </c>
@@ -1770,7 +2698,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2</v>
       </c>
@@ -1784,7 +2712,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2</v>
       </c>
@@ -1798,7 +2726,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2</v>
       </c>
@@ -1812,7 +2740,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2</v>
       </c>
@@ -1826,7 +2754,7 @@
         <v>7.7000000000000001E-5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2</v>
       </c>
@@ -1840,7 +2768,7 @@
         <v>1.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2</v>
       </c>
@@ -1854,7 +2782,7 @@
         <v>1.357E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2</v>
       </c>
@@ -1868,7 +2796,7 @@
         <v>0.18620100000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4</v>
       </c>
@@ -1882,7 +2810,7 @@
         <v>1.02E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>4</v>
       </c>
@@ -1896,7 +2824,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>4</v>
       </c>
@@ -1910,7 +2838,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>4</v>
       </c>
@@ -1924,7 +2852,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>4</v>
       </c>
@@ -1938,7 +2866,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>4</v>
       </c>
@@ -1952,7 +2880,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>4</v>
       </c>
@@ -1966,7 +2894,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4</v>
       </c>
@@ -1980,7 +2908,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>4</v>
       </c>
@@ -1994,7 +2922,7 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>4</v>
       </c>
@@ -2008,7 +2936,7 @@
         <v>1.4E-5</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>4</v>
       </c>
@@ -2022,7 +2950,7 @@
         <v>4.5000000000000003E-5</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4</v>
       </c>
@@ -2036,7 +2964,7 @@
         <v>1.6000000000000001E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4</v>
       </c>
@@ -2050,7 +2978,7 @@
         <v>5.9299999999999999E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4</v>
       </c>
@@ -2064,7 +2992,7 @@
         <v>2.1419999999999998E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4</v>
       </c>
@@ -2078,7 +3006,7 @@
         <v>7.9559999999999995E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4</v>
       </c>
@@ -2092,7 +3020,7 @@
         <v>2.8892999999999999E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4</v>
       </c>
@@ -2106,7 +3034,7 @@
         <v>0.107797</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4</v>
       </c>
@@ -2120,7 +3048,7 @@
         <v>0.40514600000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4</v>
       </c>
@@ -2134,7 +3062,7 @@
         <v>8.7999999999999998E-5</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
@@ -2148,7 +3076,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4</v>
       </c>
@@ -2162,7 +3090,7 @@
         <v>1.4E-5</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4</v>
       </c>
@@ -2176,7 +3104,7 @@
         <v>8.6200000000000003E-4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>4</v>
       </c>
@@ -2190,7 +3118,7 @@
         <v>6.5116999999999994E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -2204,7 +3132,7 @@
         <v>5.3393189999999997</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>4</v>
       </c>
@@ -2218,7 +3146,7 @@
         <v>7.7000000000000001E-5</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4</v>
       </c>
@@ -2232,7 +3160,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4</v>
       </c>
@@ -2246,7 +3174,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>4</v>
       </c>
@@ -2260,7 +3188,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>4</v>
       </c>
@@ -2274,7 +3202,7 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>4</v>
       </c>
@@ -2288,7 +3216,7 @@
         <v>4.6E-5</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>4</v>
       </c>
@@ -2302,7 +3230,7 @@
         <v>6.11E-4</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4</v>
       </c>
@@ -2316,7 +3244,7 @@
         <v>8.0510000000000009E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>4</v>
       </c>
@@ -2330,7 +3258,7 @@
         <v>0.10885499999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>8</v>
       </c>
@@ -2344,7 +3272,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>8</v>
       </c>
@@ -2358,7 +3286,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>8</v>
       </c>
@@ -2372,7 +3300,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>8</v>
       </c>
@@ -2386,7 +3314,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>8</v>
       </c>
@@ -2400,7 +3328,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>8</v>
       </c>
@@ -2414,7 +3342,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>8</v>
       </c>
@@ -2428,7 +3356,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>8</v>
       </c>
@@ -2442,7 +3370,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>8</v>
       </c>
@@ -2456,7 +3384,7 @@
         <v>3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>8</v>
       </c>
@@ -2470,7 +3398,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>8</v>
       </c>
@@ -2484,7 +3412,7 @@
         <v>2.8E-5</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>8</v>
       </c>
@@ -2498,7 +3426,7 @@
         <v>9.2999999999999997E-5</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>8</v>
       </c>
@@ -2512,7 +3440,7 @@
         <v>3.6000000000000002E-4</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>8</v>
       </c>
@@ -2526,7 +3454,7 @@
         <v>1.297E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>8</v>
       </c>
@@ -2540,7 +3468,7 @@
         <v>4.9709999999999997E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>8</v>
       </c>
@@ -2554,7 +3482,7 @@
         <v>1.7499000000000001E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>8</v>
       </c>
@@ -2568,7 +3496,7 @@
         <v>6.3252000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>8</v>
       </c>
@@ -2582,7 +3510,7 @@
         <v>0.22461</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>8</v>
       </c>
@@ -2596,7 +3524,7 @@
         <v>9.8999999999999994E-5</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>8</v>
       </c>
@@ -2610,7 +3538,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>8</v>
       </c>
@@ -2624,7 +3552,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>8</v>
       </c>
@@ -2638,7 +3566,7 @@
         <v>4.7600000000000002E-4</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>8</v>
       </c>
@@ -2652,7 +3580,7 @@
         <v>3.6138000000000003E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>8</v>
       </c>
@@ -2666,7 +3594,7 @@
         <v>2.9122119999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>8</v>
       </c>
@@ -2680,7 +3608,7 @@
         <v>1.2899999999999999E-4</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>8</v>
       </c>
@@ -2694,7 +3622,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>8</v>
       </c>
@@ -2708,7 +3636,7 @@
         <v>7.9999999999999996E-6</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>8</v>
       </c>
@@ -2722,7 +3650,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>8</v>
       </c>
@@ -2736,7 +3664,7 @@
         <v>1.4E-5</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>8</v>
       </c>
@@ -2750,7 +3678,7 @@
         <v>2.8E-5</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>8</v>
       </c>
@@ -2764,7 +3692,7 @@
         <v>3.6299999999999999E-4</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>8</v>
       </c>
@@ -2778,7 +3706,7 @@
         <v>4.9220000000000002E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>8</v>
       </c>
@@ -2794,5 +3722,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>